<commit_message>
js:biblio v5; react; images
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="384">
   <si>
     <t>id</t>
   </si>
@@ -129,9 +129,6 @@
     <t>04_js\exercicios_js\exercicioForm\formExercicio.html</t>
   </si>
   <si>
-    <t>04_js\exercicios_js\biblioteca\biblioteca-V4-add-edit\index.html</t>
-  </si>
-  <si>
     <t>front end devolpment</t>
   </si>
   <si>
@@ -747,9 +744,6 @@
     <t>js : 9-1-exercicio - callFunctions</t>
   </si>
   <si>
-    <t>library v4</t>
-  </si>
-  <si>
     <t>async random user</t>
   </si>
   <si>
@@ -1150,6 +1144,30 @@
   </si>
   <si>
     <t>02_css\12-rwd-images\rwd-image.html</t>
+  </si>
+  <si>
+    <t>front end repository</t>
+  </si>
+  <si>
+    <t>voting app</t>
+  </si>
+  <si>
+    <t>hooks</t>
+  </si>
+  <si>
+    <t>https://github.com/mario8988silva/frontEnd_project.git</t>
+  </si>
+  <si>
+    <t>library v5</t>
+  </si>
+  <si>
+    <t>04_js\exercicios_js\biblioteca\biblioteca-V5-fetch-async\index.html</t>
+  </si>
+  <si>
+    <t>05_react\1-voting-app\index.html</t>
+  </si>
+  <si>
+    <t>05_react\2-hooks\index.html</t>
   </si>
 </sst>
 </file>
@@ -1522,12 +1540,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F184"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
+      <selection pane="bottomLeft" activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1548,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1575,7 +1593,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="2" t="s">
@@ -1591,10 +1609,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="2" t="s">
@@ -1610,10 +1628,10 @@
         <v>102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="2" t="s">
@@ -1629,10 +1647,10 @@
         <v>103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="2" t="s">
@@ -1648,10 +1666,10 @@
         <v>104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="2" t="s">
@@ -1667,10 +1685,10 @@
         <v>105</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="2" t="s">
@@ -1686,10 +1704,10 @@
         <v>106</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="2" t="s">
@@ -1705,10 +1723,10 @@
         <v>107</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="2" t="s">
@@ -1724,10 +1742,10 @@
         <v>108</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="2" t="s">
@@ -1743,10 +1761,10 @@
         <v>109</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="2" t="s">
@@ -1762,10 +1780,10 @@
         <v>110</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="2" t="s">
@@ -1781,10 +1799,10 @@
         <v>111</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="2" t="s">
@@ -1800,10 +1818,10 @@
         <v>112</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="2" t="s">
@@ -1819,10 +1837,10 @@
         <v>113</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="2" t="s">
@@ -1838,10 +1856,10 @@
         <v>114</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="2" t="s">
@@ -1857,10 +1875,10 @@
         <v>115</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="2" t="s">
@@ -1876,10 +1894,10 @@
         <v>116</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="2" t="s">
@@ -1895,10 +1913,10 @@
         <v>117</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="2" t="s">
@@ -1914,10 +1932,10 @@
         <v>118</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="2" t="s">
@@ -1933,10 +1951,10 @@
         <v>119</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>6</v>
@@ -1951,10 +1969,10 @@
         <v>120</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>6</v>
@@ -1969,10 +1987,10 @@
         <v>121</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>6</v>
@@ -1987,10 +2005,10 @@
         <v>122</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>6</v>
@@ -2005,10 +2023,10 @@
         <v>123</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>6</v>
@@ -2023,10 +2041,10 @@
         <v>124</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>6</v>
@@ -2041,10 +2059,10 @@
         <v>125</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>6</v>
@@ -2059,10 +2077,10 @@
         <v>126</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>6</v>
@@ -2077,10 +2095,10 @@
         <v>127</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>6</v>
@@ -2095,10 +2113,10 @@
         <v>128</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>6</v>
@@ -2119,7 +2137,7 @@
         <v>25</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>6</v>
@@ -2141,7 +2159,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="2" t="s">
@@ -2157,10 +2175,10 @@
         <v>201</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>18</v>
@@ -2175,10 +2193,10 @@
         <v>202</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>18</v>
@@ -2193,10 +2211,10 @@
         <v>203</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>18</v>
@@ -2211,10 +2229,10 @@
         <v>204</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>18</v>
@@ -2229,10 +2247,10 @@
         <v>205</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>18</v>
@@ -2247,10 +2265,10 @@
         <v>206</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>18</v>
@@ -2265,10 +2283,10 @@
         <v>207</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>18</v>
@@ -2283,10 +2301,10 @@
         <v>208</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>18</v>
@@ -2301,10 +2319,10 @@
         <v>209</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>18</v>
@@ -2319,10 +2337,10 @@
         <v>210</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>18</v>
@@ -2337,10 +2355,10 @@
         <v>211</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>18</v>
@@ -2355,10 +2373,10 @@
         <v>212</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>18</v>
@@ -2373,10 +2391,10 @@
         <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>18</v>
@@ -2391,10 +2409,10 @@
         <v>214</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>18</v>
@@ -2409,10 +2427,10 @@
         <v>215</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>18</v>
@@ -2427,10 +2445,10 @@
         <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C50" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>18</v>
@@ -2445,10 +2463,10 @@
         <v>217</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>18</v>
@@ -2463,10 +2481,10 @@
         <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>18</v>
@@ -2481,10 +2499,10 @@
         <v>219</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>18</v>
@@ -2499,10 +2517,10 @@
         <v>220</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>18</v>
@@ -2517,10 +2535,10 @@
         <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C55" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>18</v>
@@ -2535,10 +2553,10 @@
         <v>222</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>18</v>
@@ -2553,10 +2571,10 @@
         <v>223</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>18</v>
@@ -2571,10 +2589,10 @@
         <v>224</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>18</v>
@@ -2589,10 +2607,10 @@
         <v>225</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>18</v>
@@ -2607,10 +2625,10 @@
         <v>226</v>
       </c>
       <c r="B60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>18</v>
@@ -2625,10 +2643,10 @@
         <v>227</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C61" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>18</v>
@@ -2643,10 +2661,10 @@
         <v>228</v>
       </c>
       <c r="B62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>18</v>
@@ -2661,10 +2679,10 @@
         <v>229</v>
       </c>
       <c r="B63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C63" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>18</v>
@@ -2679,10 +2697,10 @@
         <v>230</v>
       </c>
       <c r="B64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C64" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>18</v>
@@ -2697,10 +2715,10 @@
         <v>231</v>
       </c>
       <c r="B65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C65" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>18</v>
@@ -2715,10 +2733,10 @@
         <v>232</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>18</v>
@@ -2733,10 +2751,10 @@
         <v>233</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C67" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>18</v>
@@ -2751,10 +2769,10 @@
         <v>234</v>
       </c>
       <c r="B68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C68" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>18</v>
@@ -2769,10 +2787,10 @@
         <v>235</v>
       </c>
       <c r="B69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>18</v>
@@ -2787,10 +2805,10 @@
         <v>236</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>18</v>
@@ -2805,10 +2823,10 @@
         <v>237</v>
       </c>
       <c r="B71" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C71" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>18</v>
@@ -2823,10 +2841,10 @@
         <v>238</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C72" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>18</v>
@@ -2841,10 +2859,10 @@
         <v>239</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C73" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>18</v>
@@ -2859,10 +2877,10 @@
         <v>240</v>
       </c>
       <c r="B74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>18</v>
@@ -2877,10 +2895,10 @@
         <v>241</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C75" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>18</v>
@@ -2895,10 +2913,10 @@
         <v>242</v>
       </c>
       <c r="B76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>18</v>
@@ -2913,10 +2931,10 @@
         <v>243</v>
       </c>
       <c r="B77" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C77" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>18</v>
@@ -2931,10 +2949,10 @@
         <v>244</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C78" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>18</v>
@@ -2949,10 +2967,10 @@
         <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C79" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>18</v>
@@ -2967,10 +2985,10 @@
         <v>246</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C80" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>18</v>
@@ -2985,10 +3003,10 @@
         <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C81" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>18</v>
@@ -3003,10 +3021,10 @@
         <v>248</v>
       </c>
       <c r="B82" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>18</v>
@@ -3021,10 +3039,10 @@
         <v>249</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C83" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>18</v>
@@ -3039,10 +3057,10 @@
         <v>250</v>
       </c>
       <c r="B84" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C84" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>18</v>
@@ -3057,10 +3075,10 @@
         <v>251</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C85" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>18</v>
@@ -3075,10 +3093,10 @@
         <v>252</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C86" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>18</v>
@@ -3093,10 +3111,10 @@
         <v>253</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C87" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>18</v>
@@ -3111,10 +3129,10 @@
         <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C88" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>18</v>
@@ -3129,10 +3147,10 @@
         <v>255</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C89" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>18</v>
@@ -3147,10 +3165,10 @@
         <v>256</v>
       </c>
       <c r="B90" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>18</v>
@@ -3165,10 +3183,10 @@
         <v>257</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C91" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>18</v>
@@ -3183,10 +3201,10 @@
         <v>258</v>
       </c>
       <c r="B92" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C92" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>18</v>
@@ -3201,10 +3219,10 @@
         <v>259</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C93" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>18</v>
@@ -3219,10 +3237,10 @@
         <v>260</v>
       </c>
       <c r="B94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C94" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>18</v>
@@ -3237,10 +3255,10 @@
         <v>261</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C95" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>18</v>
@@ -3255,10 +3273,10 @@
         <v>262</v>
       </c>
       <c r="B96" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C96" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>18</v>
@@ -3273,10 +3291,10 @@
         <v>263</v>
       </c>
       <c r="B97" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C97" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>18</v>
@@ -3291,10 +3309,10 @@
         <v>264</v>
       </c>
       <c r="B98" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C98" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>18</v>
@@ -3309,10 +3327,10 @@
         <v>265</v>
       </c>
       <c r="B99" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C99" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>18</v>
@@ -3327,10 +3345,10 @@
         <v>266</v>
       </c>
       <c r="B100" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C100" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>18</v>
@@ -3345,10 +3363,10 @@
         <v>267</v>
       </c>
       <c r="B101" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C101" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>18</v>
@@ -3363,10 +3381,10 @@
         <v>268</v>
       </c>
       <c r="B102" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C102" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>18</v>
@@ -3381,10 +3399,10 @@
         <v>269</v>
       </c>
       <c r="B103" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>18</v>
@@ -3399,10 +3417,10 @@
         <v>270</v>
       </c>
       <c r="B104" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C104" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>18</v>
@@ -3417,10 +3435,10 @@
         <v>271</v>
       </c>
       <c r="B105" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C105" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>18</v>
@@ -3435,10 +3453,10 @@
         <v>272</v>
       </c>
       <c r="B106" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C106" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>18</v>
@@ -3453,10 +3471,10 @@
         <v>273</v>
       </c>
       <c r="B107" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C107" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>18</v>
@@ -3471,10 +3489,10 @@
         <v>274</v>
       </c>
       <c r="B108" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C108" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>18</v>
@@ -3489,10 +3507,10 @@
         <v>275</v>
       </c>
       <c r="B109" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C109" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>18</v>
@@ -3507,10 +3525,10 @@
         <v>276</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C110" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>18</v>
@@ -3525,10 +3543,10 @@
         <v>277</v>
       </c>
       <c r="B111" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C111" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>18</v>
@@ -3543,10 +3561,10 @@
         <v>278</v>
       </c>
       <c r="B112" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C112" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>18</v>
@@ -3561,10 +3579,10 @@
         <v>279</v>
       </c>
       <c r="B113" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C113" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>18</v>
@@ -3579,10 +3597,10 @@
         <v>280</v>
       </c>
       <c r="B114" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C114" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>18</v>
@@ -3597,10 +3615,10 @@
         <v>281</v>
       </c>
       <c r="B115" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>18</v>
@@ -3615,10 +3633,10 @@
         <v>282</v>
       </c>
       <c r="B116" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C116" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>18</v>
@@ -3629,7 +3647,7 @@
     </row>
     <row r="117" spans="1:6" s="4" customFormat="1">
       <c r="A117" s="2">
-        <f>SUM(A116)+1</f>
+        <f t="shared" ref="A117:A126" si="2">SUM(A116)+1</f>
         <v>283</v>
       </c>
       <c r="B117" s="4" t="s">
@@ -3639,7 +3657,7 @@
         <v>26</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>18</v>
@@ -3650,7 +3668,7 @@
     </row>
     <row r="118" spans="1:6" s="4" customFormat="1">
       <c r="A118" s="2">
-        <f>SUM(A117)+1</f>
+        <f t="shared" si="2"/>
         <v>284</v>
       </c>
       <c r="B118" s="3" t="s">
@@ -3660,7 +3678,7 @@
         <v>27</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>18</v>
@@ -3671,7 +3689,7 @@
     </row>
     <row r="119" spans="1:6" s="4" customFormat="1">
       <c r="A119" s="2">
-        <f>SUM(A118)+1</f>
+        <f t="shared" si="2"/>
         <v>285</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -3681,7 +3699,7 @@
         <v>28</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>18</v>
@@ -3692,7 +3710,7 @@
     </row>
     <row r="120" spans="1:6" s="4" customFormat="1">
       <c r="A120" s="2">
-        <f>SUM(A119)+1</f>
+        <f t="shared" si="2"/>
         <v>286</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -3702,7 +3720,7 @@
         <v>29</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>18</v>
@@ -3713,7 +3731,7 @@
     </row>
     <row r="121" spans="1:6" s="4" customFormat="1">
       <c r="A121" s="2">
-        <f>SUM(A120)+1</f>
+        <f t="shared" si="2"/>
         <v>287</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -3723,7 +3741,7 @@
         <v>30</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>18</v>
@@ -3734,7 +3752,7 @@
     </row>
     <row r="122" spans="1:6" s="4" customFormat="1">
       <c r="A122" s="2">
-        <f>SUM(A121)+1</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -3744,7 +3762,7 @@
         <v>31</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>18</v>
@@ -3755,7 +3773,7 @@
     </row>
     <row r="123" spans="1:6" s="4" customFormat="1">
       <c r="A123" s="2">
-        <f>SUM(A122)+1</f>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -3765,7 +3783,7 @@
         <v>32</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>18</v>
@@ -3776,7 +3794,7 @@
     </row>
     <row r="124" spans="1:6" s="4" customFormat="1">
       <c r="A124" s="2">
-        <f>SUM(A123)+1</f>
+        <f t="shared" si="2"/>
         <v>290</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -3786,7 +3804,7 @@
         <v>33</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>18</v>
@@ -3797,7 +3815,7 @@
     </row>
     <row r="125" spans="1:6" s="4" customFormat="1">
       <c r="A125" s="2">
-        <f>SUM(A124)+1</f>
+        <f t="shared" si="2"/>
         <v>291</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -3807,7 +3825,7 @@
         <v>34</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>18</v>
@@ -3818,7 +3836,7 @@
     </row>
     <row r="126" spans="1:6" s="4" customFormat="1">
       <c r="A126" s="2">
-        <f>SUM(A125)+1</f>
+        <f t="shared" si="2"/>
         <v>292</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -3828,7 +3846,7 @@
         <v>35</v>
       </c>
       <c r="D126" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>18</v>
@@ -3847,14 +3865,14 @@
         <v>300</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D128" s="10"/>
       <c r="E128" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>24</v>
@@ -3866,13 +3884,13 @@
         <v>301</v>
       </c>
       <c r="B129" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C129" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>22</v>
@@ -3884,13 +3902,13 @@
         <v>302</v>
       </c>
       <c r="B130" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C130" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>22</v>
@@ -3902,13 +3920,13 @@
         <v>303</v>
       </c>
       <c r="B131" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C131" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>22</v>
@@ -3920,13 +3938,13 @@
         <v>304</v>
       </c>
       <c r="B132" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C132" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>22</v>
@@ -3938,13 +3956,13 @@
         <v>305</v>
       </c>
       <c r="B133" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C133" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>22</v>
@@ -3956,13 +3974,13 @@
         <v>306</v>
       </c>
       <c r="B134" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C134" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>22</v>
@@ -3974,13 +3992,13 @@
         <v>307</v>
       </c>
       <c r="B135" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C135" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>22</v>
@@ -3992,13 +4010,13 @@
         <v>308</v>
       </c>
       <c r="B136" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C136" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>22</v>
@@ -4010,13 +4028,13 @@
         <v>309</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C137" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>22</v>
@@ -4028,13 +4046,13 @@
         <v>310</v>
       </c>
       <c r="B138" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C138" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>22</v>
@@ -4046,13 +4064,13 @@
         <v>311</v>
       </c>
       <c r="B139" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C139" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>22</v>
@@ -4064,13 +4082,13 @@
         <v>312</v>
       </c>
       <c r="B140" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C140" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>22</v>
@@ -4082,13 +4100,13 @@
         <v>313</v>
       </c>
       <c r="B141" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C141" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>22</v>
@@ -4100,13 +4118,13 @@
         <v>314</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>22</v>
@@ -4118,13 +4136,13 @@
         <v>315</v>
       </c>
       <c r="B143" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C143" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>22</v>
@@ -4132,17 +4150,17 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="2">
-        <f t="shared" ref="A144:A175" si="2">SUM(A143)+1</f>
+        <f t="shared" ref="A144:A175" si="3">SUM(A143)+1</f>
         <v>316</v>
       </c>
       <c r="B144" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C144" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>22</v>
@@ -4150,17 +4168,17 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>317</v>
       </c>
       <c r="B145" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C145" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>22</v>
@@ -4168,17 +4186,17 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>318</v>
       </c>
       <c r="B146" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C146" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>22</v>
@@ -4186,17 +4204,17 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>319</v>
       </c>
       <c r="B147" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C147" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>22</v>
@@ -4204,17 +4222,17 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>320</v>
       </c>
       <c r="B148" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C148" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>22</v>
@@ -4233,7 +4251,7 @@
         <v>23</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D150" s="10"/>
       <c r="E150" s="2" t="s">
@@ -4249,10 +4267,10 @@
         <v>401</v>
       </c>
       <c r="B151" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C151" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>19</v>
@@ -4263,14 +4281,14 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>402</v>
       </c>
       <c r="B152" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C152" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>19</v>
@@ -4281,14 +4299,14 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>403</v>
       </c>
       <c r="B153" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C153" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>19</v>
@@ -4299,14 +4317,14 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>404</v>
       </c>
       <c r="B154" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C154" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>19</v>
@@ -4317,14 +4335,14 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>405</v>
       </c>
       <c r="B155" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C155" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>19</v>
@@ -4335,14 +4353,14 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>406</v>
       </c>
       <c r="B156" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C156" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>19</v>
@@ -4353,14 +4371,14 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>407</v>
       </c>
       <c r="B157" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C157" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>19</v>
@@ -4371,14 +4389,14 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>408</v>
       </c>
       <c r="B158" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C158" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>19</v>
@@ -4389,14 +4407,14 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>409</v>
       </c>
       <c r="B159" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C159" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>19</v>
@@ -4407,14 +4425,14 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>410</v>
       </c>
       <c r="B160" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C160" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>19</v>
@@ -4425,14 +4443,14 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>411</v>
       </c>
       <c r="B161" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C161" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>19</v>
@@ -4443,14 +4461,14 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>412</v>
       </c>
       <c r="B162" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C162" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>19</v>
@@ -4461,14 +4479,14 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>413</v>
       </c>
       <c r="B163" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C163" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>19</v>
@@ -4479,14 +4497,14 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>414</v>
       </c>
       <c r="B164" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C164" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>19</v>
@@ -4497,14 +4515,14 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>415</v>
       </c>
       <c r="B165" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C165" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>19</v>
@@ -4515,14 +4533,14 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>416</v>
       </c>
       <c r="B166" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C166" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>19</v>
@@ -4533,14 +4551,14 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>417</v>
       </c>
       <c r="B167" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C167" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>19</v>
@@ -4551,14 +4569,14 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>418</v>
       </c>
       <c r="B168" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C168" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>19</v>
@@ -4569,14 +4587,14 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>419</v>
       </c>
       <c r="B169" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C169" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E169" s="2" t="s">
         <v>19</v>
@@ -4587,14 +4605,14 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>420</v>
       </c>
       <c r="B170" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C170" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>19</v>
@@ -4609,10 +4627,10 @@
         <v>421</v>
       </c>
       <c r="B171" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C171" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>19</v>
@@ -4627,10 +4645,10 @@
         <v>422</v>
       </c>
       <c r="B172" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C172" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E172" s="2" t="s">
         <v>19</v>
@@ -4641,14 +4659,14 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>423</v>
       </c>
       <c r="B173" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C173" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>19</v>
@@ -4659,7 +4677,7 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>424</v>
       </c>
       <c r="B174" s="4" t="s">
@@ -4669,7 +4687,7 @@
         <v>36</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>19</v>
@@ -4680,17 +4698,17 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>425</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>243</v>
+        <v>380</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>37</v>
+        <v>381</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E175" s="2" t="s">
         <v>19</v>
@@ -4705,13 +4723,13 @@
         <v>426</v>
       </c>
       <c r="B176" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D176" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="C176" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D176" s="10" t="s">
-        <v>246</v>
       </c>
       <c r="E176" s="2" t="s">
         <v>19</v>
@@ -4730,72 +4748,127 @@
         <v>500</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D178" s="10"/>
       <c r="E178" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
-      <c r="B179"/>
-    </row>
-    <row r="180" spans="1:6">
-      <c r="B180"/>
-    </row>
-    <row r="181" spans="1:6" ht="17.25">
+    <row r="179" spans="1:6" s="4" customFormat="1">
+      <c r="A179" s="2">
+        <f>SUM(A178)+1</f>
+        <v>501</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D179" s="10"/>
+      <c r="E179" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" s="4" customFormat="1">
+      <c r="A180" s="2">
+        <f t="shared" ref="A180:A181" si="4">SUM(A179)+1</f>
+        <v>502</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="D180" s="10"/>
+      <c r="E180" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181" s="2">
+        <f t="shared" si="4"/>
+        <v>503</v>
+      </c>
+      <c r="B181"/>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="B182"/>
+    </row>
+    <row r="183" spans="1:6" ht="17.25">
+      <c r="A183" s="2">
         <v>600</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B183" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C183" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D183" s="10"/>
+      <c r="E183" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C181" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D181" s="10"/>
-      <c r="E181" s="2" t="s">
+      <c r="F183" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="17.25">
+      <c r="A184" s="2">
+        <f>SUM(A183)+1</f>
+        <v>601</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="2">
+        <f>SUM(A184)+1</f>
+        <v>602</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C185" s="7"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F185" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F181" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
-      <c r="A182" s="2">
-        <f>SUM(A181)+1</f>
-        <v>601</v>
-      </c>
-      <c r="B182" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C182" s="7"/>
-      <c r="D182" s="10"/>
-      <c r="E182" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F182" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6">
-      <c r="B183"/>
-    </row>
-    <row r="184" spans="1:6">
-      <c r="B184"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C181" r:id="rId1"/>
+    <hyperlink ref="C183" r:id="rId1"/>
+    <hyperlink ref="C184" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>